<commit_message>
Overall check of the functions
</commit_message>
<xml_diff>
--- a/00 - BaseSpreadSheet.xlsx
+++ b/00 - BaseSpreadSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cristofer/Documents/07 - Software/00 - Projetos/VBA_PumpPerformance/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petrobrasbr-my.sharepoint.com/personal/cristofer_petrobras_com_br/Documents/10 - GitHub/vba-pump-performance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47DA11C6-38AB-6649-AEA5-ECC61A213ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{47DA11C6-38AB-6649-AEA5-ECC61A213ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3491BF4E-6D6A-4900-AEDF-42AB7ABB49AF}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="570" yWindow="-15630" windowWidth="18300" windowHeight="14670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GettingStarted" sheetId="2" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="226">
   <si>
     <t>required filling field</t>
   </si>
@@ -689,18 +689,12 @@
     <t>$f$21</t>
   </si>
   <si>
-    <t>Tool_ModulesImport.bas</t>
-  </si>
-  <si>
     <t>Pump.cls</t>
   </si>
   <si>
     <t>TestPoint.cls</t>
   </si>
   <si>
-    <t>a4_PumpPerformanceMain.bas</t>
-  </si>
-  <si>
     <t>Tool_OptmizationEnd.bas</t>
   </si>
   <si>
@@ -734,9 +728,6 @@
     <t>a3_RunPerformance.bas</t>
   </si>
   <si>
-    <t>Module1.bas</t>
-  </si>
-  <si>
     <t>a2_ClonePump.bas</t>
   </si>
   <si>
@@ -807,6 +798,21 @@
   </si>
   <si>
     <t>Cells coloured :</t>
+  </si>
+  <si>
+    <t>a5_ResetCalcFields.bas</t>
+  </si>
+  <si>
+    <t>a6_ResetMain.bas</t>
+  </si>
+  <si>
+    <t>a7_Report.bas</t>
+  </si>
+  <si>
+    <t>a8_WordReport.bas</t>
+  </si>
+  <si>
+    <t>a4_PerformanceMain.bas</t>
   </si>
 </sst>
 </file>
@@ -1901,29 +1907,29 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="16384" width="10.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C9" s="2"/>
       <c r="D9" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C11" s="3"/>
       <c r="D11" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C13" s="4"/>
       <c r="D13" s="1" t="s">
         <v>1</v>
@@ -1942,24 +1948,24 @@
   <dimension ref="B1:L132"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="107" zoomScaleNormal="150" zoomScaleSheetLayoutView="84" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:E6"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="1.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.6328125" style="1" customWidth="1"/>
     <col min="2" max="2" width="4" style="5" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.1796875" style="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" customWidth="1"/>
-    <col min="5" max="10" width="11.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="1.83203125" style="1" customWidth="1"/>
-    <col min="12" max="16" width="10.83203125" style="1"/>
-    <col min="17" max="17" width="18.6640625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.83203125" style="1"/>
+    <col min="5" max="10" width="11.6328125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="1.81640625" style="1" customWidth="1"/>
+    <col min="12" max="16" width="10.81640625" style="1"/>
+    <col min="17" max="17" width="18.6328125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:11" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="6"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -1971,7 +1977,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="8"/>
     </row>
-    <row r="3" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="9"/>
       <c r="C3" s="105" t="s">
         <v>3</v>
@@ -1985,7 +1991,7 @@
       <c r="J3" s="105"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="2:11" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="11"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
@@ -1997,13 +2003,13 @@
       <c r="J4" s="13"/>
       <c r="K4" s="14"/>
     </row>
-    <row r="5" spans="2:11" ht="4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11" ht="4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="15"/>
       <c r="C5" s="16"/>
       <c r="D5" s="16"/>
       <c r="K5" s="17"/>
     </row>
-    <row r="6" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="18">
         <v>1</v>
       </c>
@@ -2021,7 +2027,7 @@
       <c r="J6" s="20"/>
       <c r="K6" s="17"/>
     </row>
-    <row r="7" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="18">
         <f>B6+1</f>
         <v>2</v>
@@ -2040,7 +2046,7 @@
       <c r="J7" s="20"/>
       <c r="K7" s="17"/>
     </row>
-    <row r="8" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="18">
         <f t="shared" ref="B8:B69" si="0">B7+1</f>
         <v>3</v>
@@ -2059,7 +2065,7 @@
       <c r="J8" s="20"/>
       <c r="K8" s="17"/>
     </row>
-    <row r="9" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="18">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2078,7 +2084,7 @@
       <c r="J9" s="20"/>
       <c r="K9" s="17"/>
     </row>
-    <row r="10" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="18">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2095,7 +2101,7 @@
       <c r="J10" s="20"/>
       <c r="K10" s="17"/>
     </row>
-    <row r="11" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="18">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2112,7 +2118,7 @@
       <c r="J11" s="20"/>
       <c r="K11" s="17"/>
     </row>
-    <row r="12" spans="2:11" ht="4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" ht="4" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="18">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2127,7 +2133,7 @@
       <c r="J12" s="21"/>
       <c r="K12" s="14"/>
     </row>
-    <row r="13" spans="2:11" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="18">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2146,7 +2152,7 @@
       <c r="J13" s="23"/>
       <c r="K13" s="25"/>
     </row>
-    <row r="14" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="18">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2172,7 +2178,7 @@
       </c>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="18">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2194,7 +2200,7 @@
       <c r="J15" s="36"/>
       <c r="K15" s="17"/>
     </row>
-    <row r="16" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="18">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2216,7 +2222,7 @@
       <c r="J16" s="36"/>
       <c r="K16" s="17"/>
     </row>
-    <row r="17" spans="2:11" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B17" s="18">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2231,7 +2237,7 @@
       <c r="J17" s="36"/>
       <c r="K17" s="17"/>
     </row>
-    <row r="18" spans="2:11" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="18">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2252,7 +2258,7 @@
       <c r="J18" s="36"/>
       <c r="K18" s="17"/>
     </row>
-    <row r="19" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="18">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2275,7 +2281,7 @@
       <c r="J19" s="36"/>
       <c r="K19" s="17"/>
     </row>
-    <row r="20" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="18">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2291,7 +2297,7 @@
       <c r="G20" s="43"/>
       <c r="K20" s="17"/>
     </row>
-    <row r="21" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="18">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2307,7 +2313,7 @@
       <c r="G21" s="43"/>
       <c r="K21" s="17"/>
     </row>
-    <row r="22" spans="2:11" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B22" s="18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2322,7 +2328,7 @@
       <c r="J22" s="21"/>
       <c r="K22" s="14"/>
     </row>
-    <row r="23" spans="2:11" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="18">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2341,7 +2347,7 @@
       <c r="J23" s="23"/>
       <c r="K23" s="25"/>
     </row>
-    <row r="24" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="18">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2360,7 +2366,7 @@
       <c r="J24" s="48"/>
       <c r="K24" s="8"/>
     </row>
-    <row r="25" spans="2:11" ht="24" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B25" s="18">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2391,7 +2397,7 @@
       </c>
       <c r="K25" s="53"/>
     </row>
-    <row r="26" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="18">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2422,7 +2428,7 @@
       </c>
       <c r="K26" s="17"/>
     </row>
-    <row r="27" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="18">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2450,7 +2456,7 @@
       </c>
       <c r="K27" s="17"/>
     </row>
-    <row r="28" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="18">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2461,7 +2467,7 @@
       <c r="D28" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="E28" s="55"/>
+      <c r="E28" s="58"/>
       <c r="F28" s="56"/>
       <c r="G28" s="56"/>
       <c r="H28" s="98" t="str">
@@ -2478,7 +2484,7 @@
       </c>
       <c r="K28" s="17"/>
     </row>
-    <row r="29" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="18">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2505,7 +2511,7 @@
       </c>
       <c r="K29" s="17"/>
     </row>
-    <row r="30" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="18">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2524,7 +2530,7 @@
       <c r="J30" s="57"/>
       <c r="K30" s="17"/>
     </row>
-    <row r="31" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="18">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2543,7 +2549,7 @@
       <c r="J31" s="57"/>
       <c r="K31" s="17"/>
     </row>
-    <row r="32" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" s="18">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -2574,7 +2580,7 @@
       </c>
       <c r="K32" s="17"/>
     </row>
-    <row r="33" spans="2:12" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:12" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B33" s="18">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2589,7 +2595,7 @@
       <c r="J33" s="21"/>
       <c r="K33" s="14"/>
     </row>
-    <row r="34" spans="2:12" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:12" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B34" s="18">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -2606,7 +2612,7 @@
       <c r="J34" s="23"/>
       <c r="K34" s="25"/>
     </row>
-    <row r="35" spans="2:12" ht="24" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:12" ht="18" x14ac:dyDescent="0.35">
       <c r="B35" s="18">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2637,7 +2643,7 @@
       </c>
       <c r="K35" s="64"/>
     </row>
-    <row r="36" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="18">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2654,7 +2660,7 @@
       <c r="J36" s="20"/>
       <c r="K36" s="17"/>
     </row>
-    <row r="37" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B37" s="18">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2671,7 +2677,7 @@
       <c r="J37" s="67"/>
       <c r="K37" s="17"/>
     </row>
-    <row r="38" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B38" s="18">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -2688,7 +2694,7 @@
       <c r="J38" s="67"/>
       <c r="K38" s="17"/>
     </row>
-    <row r="39" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B39" s="18">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -2705,7 +2711,7 @@
       <c r="J39" s="67"/>
       <c r="K39" s="17"/>
     </row>
-    <row r="40" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B40" s="18">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -2722,7 +2728,7 @@
       <c r="J40" s="67"/>
       <c r="K40" s="17"/>
     </row>
-    <row r="41" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B41" s="18">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -2739,7 +2745,7 @@
       <c r="J41" s="20"/>
       <c r="K41" s="17"/>
     </row>
-    <row r="42" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B42" s="18">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -2756,7 +2762,7 @@
       <c r="J42" s="67"/>
       <c r="K42" s="17"/>
     </row>
-    <row r="43" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B43" s="18">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -2773,7 +2779,7 @@
       <c r="J43" s="67"/>
       <c r="K43" s="17"/>
     </row>
-    <row r="44" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B44" s="18">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -2790,7 +2796,7 @@
       <c r="J44" s="67"/>
       <c r="K44" s="17"/>
     </row>
-    <row r="45" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B45" s="18">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -2807,7 +2813,7 @@
       <c r="J45" s="67"/>
       <c r="K45" s="17"/>
     </row>
-    <row r="46" spans="2:12" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:12" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B46" s="18">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -2822,7 +2828,7 @@
       <c r="J46" s="21"/>
       <c r="K46" s="14"/>
     </row>
-    <row r="47" spans="2:12" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:12" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B47" s="18">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -2839,7 +2845,7 @@
       <c r="J47" s="23"/>
       <c r="K47" s="25"/>
     </row>
-    <row r="48" spans="2:12" ht="24" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:12" ht="18" x14ac:dyDescent="0.35">
       <c r="B48" s="18">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -2871,7 +2877,7 @@
       <c r="K48" s="64"/>
       <c r="L48" s="70"/>
     </row>
-    <row r="49" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B49" s="18">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -2890,7 +2896,7 @@
       <c r="J49" s="72"/>
       <c r="K49" s="17"/>
     </row>
-    <row r="50" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B50" s="18">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -2909,7 +2915,7 @@
       <c r="J50" s="72"/>
       <c r="K50" s="17"/>
     </row>
-    <row r="51" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B51" s="18">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -2928,7 +2934,7 @@
       <c r="J51" s="72"/>
       <c r="K51" s="17"/>
     </row>
-    <row r="52" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B52" s="18">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -2947,7 +2953,7 @@
       <c r="J52" s="41"/>
       <c r="K52" s="17"/>
     </row>
-    <row r="53" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B53" s="18">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -2966,7 +2972,7 @@
       <c r="J53" s="72"/>
       <c r="K53" s="17"/>
     </row>
-    <row r="54" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B54" s="18">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -2985,7 +2991,7 @@
       <c r="J54" s="41"/>
       <c r="K54" s="17"/>
     </row>
-    <row r="55" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B55" s="18">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -3004,7 +3010,7 @@
       <c r="J55" s="59"/>
       <c r="K55" s="17"/>
     </row>
-    <row r="56" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B56" s="18">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -3023,7 +3029,7 @@
       <c r="J56" s="103"/>
       <c r="K56" s="17"/>
     </row>
-    <row r="57" spans="2:12" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:12" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B57" s="18">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -3038,7 +3044,7 @@
       <c r="J57" s="21"/>
       <c r="K57" s="14"/>
     </row>
-    <row r="58" spans="2:12" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:12" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B58" s="18">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -3055,7 +3061,7 @@
       <c r="J58" s="23"/>
       <c r="K58" s="25"/>
     </row>
-    <row r="59" spans="2:12" ht="24" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:12" ht="18" x14ac:dyDescent="0.35">
       <c r="B59" s="18">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -3087,7 +3093,7 @@
       <c r="K59" s="64"/>
       <c r="L59" s="70"/>
     </row>
-    <row r="60" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B60" s="18">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -3106,7 +3112,7 @@
       <c r="J60" s="74"/>
       <c r="K60" s="17"/>
     </row>
-    <row r="61" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B61" s="18">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -3125,7 +3131,7 @@
       <c r="J61" s="74"/>
       <c r="K61" s="17"/>
     </row>
-    <row r="62" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B62" s="18">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -3144,7 +3150,7 @@
       <c r="J62" s="74"/>
       <c r="K62" s="17"/>
     </row>
-    <row r="63" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B63" s="18">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -3163,7 +3169,7 @@
       <c r="J63" s="74"/>
       <c r="K63" s="17"/>
     </row>
-    <row r="64" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B64" s="18">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -3182,7 +3188,7 @@
       <c r="J64" s="75"/>
       <c r="K64" s="17"/>
     </row>
-    <row r="65" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B65" s="18">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -3201,7 +3207,7 @@
       <c r="J65" s="74"/>
       <c r="K65" s="17"/>
     </row>
-    <row r="66" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B66" s="18">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -3220,7 +3226,7 @@
       <c r="J66" s="74"/>
       <c r="K66" s="17"/>
     </row>
-    <row r="67" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B67" s="18">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -3239,7 +3245,7 @@
       <c r="J67" s="74"/>
       <c r="K67" s="17"/>
     </row>
-    <row r="68" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B68" s="18">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -3258,7 +3264,7 @@
       <c r="J68" s="74"/>
       <c r="K68" s="17"/>
     </row>
-    <row r="69" spans="2:11" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:11" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B69" s="18">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -3273,7 +3279,7 @@
       <c r="J69" s="20"/>
       <c r="K69" s="17"/>
     </row>
-    <row r="70" spans="2:11" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:11" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B70" s="76">
         <v>1</v>
       </c>
@@ -3289,7 +3295,7 @@
       <c r="J70" s="23"/>
       <c r="K70" s="25"/>
     </row>
-    <row r="71" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B71" s="77">
         <f t="shared" ref="B71:B132" si="1">B70+1</f>
         <v>2</v>
@@ -3304,7 +3310,7 @@
       <c r="J71" s="48"/>
       <c r="K71" s="8"/>
     </row>
-    <row r="72" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B72" s="77">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -3323,7 +3329,7 @@
       <c r="J72" s="20"/>
       <c r="K72" s="17"/>
     </row>
-    <row r="73" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B73" s="77">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -3350,7 +3356,7 @@
       </c>
       <c r="K73" s="17"/>
     </row>
-    <row r="74" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B74" s="77">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -3369,7 +3375,7 @@
       <c r="J74" s="67"/>
       <c r="K74" s="17"/>
     </row>
-    <row r="75" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B75" s="77">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -3388,7 +3394,7 @@
       <c r="J75" s="67"/>
       <c r="K75" s="17"/>
     </row>
-    <row r="76" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B76" s="77">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -3407,7 +3413,7 @@
       <c r="J76" s="67"/>
       <c r="K76" s="17"/>
     </row>
-    <row r="77" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B77" s="77">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -3424,7 +3430,7 @@
       <c r="J77" s="20"/>
       <c r="K77" s="17"/>
     </row>
-    <row r="78" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B78" s="77">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -3441,7 +3447,7 @@
       <c r="J78" s="20"/>
       <c r="K78" s="17"/>
     </row>
-    <row r="79" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B79" s="77">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -3458,7 +3464,7 @@
       <c r="J79" s="20"/>
       <c r="K79" s="17"/>
     </row>
-    <row r="80" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B80" s="77">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -3475,7 +3481,7 @@
       <c r="J80" s="20"/>
       <c r="K80" s="17"/>
     </row>
-    <row r="81" spans="2:11" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:11" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B81" s="77">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -3490,7 +3496,7 @@
       <c r="J81" s="21"/>
       <c r="K81" s="14"/>
     </row>
-    <row r="82" spans="2:11" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:11" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B82" s="77">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -3507,7 +3513,7 @@
       <c r="J82" s="48"/>
       <c r="K82" s="8"/>
     </row>
-    <row r="83" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B83" s="83">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -3522,7 +3528,7 @@
       <c r="J83" s="48"/>
       <c r="K83" s="8"/>
     </row>
-    <row r="84" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B84" s="83">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -3537,7 +3543,7 @@
       <c r="J84" s="20"/>
       <c r="K84" s="17"/>
     </row>
-    <row r="85" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B85" s="83">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -3552,7 +3558,7 @@
       <c r="J85" s="20"/>
       <c r="K85" s="17"/>
     </row>
-    <row r="86" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B86" s="83">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -3567,7 +3573,7 @@
       <c r="J86" s="20"/>
       <c r="K86" s="17"/>
     </row>
-    <row r="87" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B87" s="83">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -3582,7 +3588,7 @@
       <c r="J87" s="20"/>
       <c r="K87" s="17"/>
     </row>
-    <row r="88" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B88" s="83">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -3597,7 +3603,7 @@
       <c r="J88" s="20"/>
       <c r="K88" s="17"/>
     </row>
-    <row r="89" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B89" s="83">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -3612,7 +3618,7 @@
       <c r="J89" s="20"/>
       <c r="K89" s="17"/>
     </row>
-    <row r="90" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B90" s="83">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -3627,7 +3633,7 @@
       <c r="J90" s="20"/>
       <c r="K90" s="17"/>
     </row>
-    <row r="91" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B91" s="83">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -3642,7 +3648,7 @@
       <c r="J91" s="20"/>
       <c r="K91" s="17"/>
     </row>
-    <row r="92" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B92" s="83">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -3657,7 +3663,7 @@
       <c r="J92" s="20"/>
       <c r="K92" s="17"/>
     </row>
-    <row r="93" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B93" s="83">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -3672,7 +3678,7 @@
       <c r="J93" s="20"/>
       <c r="K93" s="17"/>
     </row>
-    <row r="94" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B94" s="83">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -3687,7 +3693,7 @@
       <c r="J94" s="20"/>
       <c r="K94" s="17"/>
     </row>
-    <row r="95" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B95" s="83">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -3702,7 +3708,7 @@
       <c r="J95" s="20"/>
       <c r="K95" s="17"/>
     </row>
-    <row r="96" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B96" s="83">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -3717,7 +3723,7 @@
       <c r="J96" s="20"/>
       <c r="K96" s="17"/>
     </row>
-    <row r="97" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B97" s="83">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -3732,7 +3738,7 @@
       <c r="J97" s="20"/>
       <c r="K97" s="17"/>
     </row>
-    <row r="98" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B98" s="83">
         <f t="shared" si="1"/>
         <v>29</v>
@@ -3747,7 +3753,7 @@
       <c r="J98" s="20"/>
       <c r="K98" s="17"/>
     </row>
-    <row r="99" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B99" s="83">
         <f t="shared" si="1"/>
         <v>30</v>
@@ -3762,7 +3768,7 @@
       <c r="J99" s="20"/>
       <c r="K99" s="17"/>
     </row>
-    <row r="100" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B100" s="83">
         <f t="shared" si="1"/>
         <v>31</v>
@@ -3777,7 +3783,7 @@
       <c r="J100" s="20"/>
       <c r="K100" s="17"/>
     </row>
-    <row r="101" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B101" s="83">
         <f t="shared" si="1"/>
         <v>32</v>
@@ -3792,7 +3798,7 @@
       <c r="J101" s="20"/>
       <c r="K101" s="17"/>
     </row>
-    <row r="102" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B102" s="83">
         <f t="shared" si="1"/>
         <v>33</v>
@@ -3807,7 +3813,7 @@
       <c r="J102" s="20"/>
       <c r="K102" s="17"/>
     </row>
-    <row r="103" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B103" s="83">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -3822,7 +3828,7 @@
       <c r="J103" s="20"/>
       <c r="K103" s="17"/>
     </row>
-    <row r="104" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B104" s="83">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -3837,7 +3843,7 @@
       <c r="J104" s="20"/>
       <c r="K104" s="17"/>
     </row>
-    <row r="105" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B105" s="83">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -3852,7 +3858,7 @@
       <c r="J105" s="20"/>
       <c r="K105" s="17"/>
     </row>
-    <row r="106" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B106" s="83">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -3867,7 +3873,7 @@
       <c r="J106" s="20"/>
       <c r="K106" s="17"/>
     </row>
-    <row r="107" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B107" s="83">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -3882,7 +3888,7 @@
       <c r="J107" s="20"/>
       <c r="K107" s="17"/>
     </row>
-    <row r="108" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B108" s="83">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -3897,7 +3903,7 @@
       <c r="J108" s="20"/>
       <c r="K108" s="17"/>
     </row>
-    <row r="109" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B109" s="83">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -3912,7 +3918,7 @@
       <c r="J109" s="20"/>
       <c r="K109" s="17"/>
     </row>
-    <row r="110" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B110" s="83">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -3927,7 +3933,7 @@
       <c r="J110" s="20"/>
       <c r="K110" s="17"/>
     </row>
-    <row r="111" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B111" s="83">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -3942,7 +3948,7 @@
       <c r="J111" s="87"/>
       <c r="K111" s="17"/>
     </row>
-    <row r="112" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B112" s="83">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -3957,7 +3963,7 @@
       <c r="J112" s="20"/>
       <c r="K112" s="17"/>
     </row>
-    <row r="113" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B113" s="83">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -3972,7 +3978,7 @@
       <c r="J113" s="20"/>
       <c r="K113" s="17"/>
     </row>
-    <row r="114" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B114" s="83">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -3987,7 +3993,7 @@
       <c r="J114" s="20"/>
       <c r="K114" s="17"/>
     </row>
-    <row r="115" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B115" s="83">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -3995,7 +4001,7 @@
       <c r="C115" s="43"/>
       <c r="K115" s="17"/>
     </row>
-    <row r="116" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B116" s="83">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -4003,7 +4009,7 @@
       <c r="C116" s="43"/>
       <c r="K116" s="17"/>
     </row>
-    <row r="117" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B117" s="83">
         <f t="shared" si="1"/>
         <v>48</v>
@@ -4011,7 +4017,7 @@
       <c r="C117" s="43"/>
       <c r="K117" s="17"/>
     </row>
-    <row r="118" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B118" s="83">
         <f t="shared" si="1"/>
         <v>49</v>
@@ -4019,7 +4025,7 @@
       <c r="C118" s="43"/>
       <c r="K118" s="17"/>
     </row>
-    <row r="119" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B119" s="83">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -4027,7 +4033,7 @@
       <c r="C119" s="43"/>
       <c r="K119" s="17"/>
     </row>
-    <row r="120" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B120" s="83">
         <f t="shared" si="1"/>
         <v>51</v>
@@ -4035,7 +4041,7 @@
       <c r="C120" s="43"/>
       <c r="K120" s="17"/>
     </row>
-    <row r="121" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B121" s="83">
         <f t="shared" si="1"/>
         <v>52</v>
@@ -4043,7 +4049,7 @@
       <c r="C121" s="43"/>
       <c r="K121" s="17"/>
     </row>
-    <row r="122" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B122" s="83">
         <f t="shared" si="1"/>
         <v>53</v>
@@ -4051,7 +4057,7 @@
       <c r="C122" s="43"/>
       <c r="K122" s="17"/>
     </row>
-    <row r="123" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B123" s="83">
         <f t="shared" si="1"/>
         <v>54</v>
@@ -4059,7 +4065,7 @@
       <c r="C123" s="43"/>
       <c r="K123" s="17"/>
     </row>
-    <row r="124" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B124" s="83">
         <f t="shared" si="1"/>
         <v>55</v>
@@ -4067,7 +4073,7 @@
       <c r="C124" s="43"/>
       <c r="K124" s="17"/>
     </row>
-    <row r="125" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B125" s="83">
         <f t="shared" si="1"/>
         <v>56</v>
@@ -4075,7 +4081,7 @@
       <c r="C125" s="43"/>
       <c r="K125" s="17"/>
     </row>
-    <row r="126" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B126" s="83">
         <f t="shared" si="1"/>
         <v>57</v>
@@ -4083,7 +4089,7 @@
       <c r="C126" s="43"/>
       <c r="K126" s="17"/>
     </row>
-    <row r="127" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B127" s="83">
         <f t="shared" si="1"/>
         <v>58</v>
@@ -4091,7 +4097,7 @@
       <c r="C127" s="43"/>
       <c r="K127" s="17"/>
     </row>
-    <row r="128" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B128" s="83">
         <f t="shared" si="1"/>
         <v>59</v>
@@ -4099,7 +4105,7 @@
       <c r="C128" s="43"/>
       <c r="K128" s="17"/>
     </row>
-    <row r="129" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B129" s="83">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -4107,7 +4113,7 @@
       <c r="C129" s="43"/>
       <c r="K129" s="17"/>
     </row>
-    <row r="130" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B130" s="83">
         <f t="shared" si="1"/>
         <v>61</v>
@@ -4115,7 +4121,7 @@
       <c r="C130" s="43"/>
       <c r="K130" s="17"/>
     </row>
-    <row r="131" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B131" s="83">
         <f t="shared" si="1"/>
         <v>62</v>
@@ -4124,7 +4130,7 @@
       <c r="J131" s="88"/>
       <c r="K131" s="17"/>
     </row>
-    <row r="132" spans="2:11" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:11" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B132" s="89">
         <f t="shared" si="1"/>
         <v>63</v>
@@ -4223,22 +4229,22 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33:I34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.83203125" style="91" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.33203125" style="91" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" style="91" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" style="91" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="91" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="4.1640625" style="91" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="91"/>
+    <col min="1" max="1" width="25.81640625" style="91" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.36328125" style="91" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.36328125" style="91" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" style="91" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" style="91" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="4.1796875" style="91" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.81640625" style="91"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="91" t="str">
         <f t="shared" ref="A1:A47" si="0">"='"&amp;$D1&amp;"'!"&amp;$E1</f>
         <v>='InputTestData'!$J$16</v>
@@ -4266,7 +4272,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$J$17</v>
@@ -4294,7 +4300,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$J$18</v>
@@ -4322,7 +4328,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$J$19</v>
@@ -4350,7 +4356,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$C$84</v>
@@ -4378,7 +4384,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$J$131</v>
@@ -4406,7 +4412,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$J$111</v>
@@ -4434,7 +4440,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$E$19</v>
@@ -4462,7 +4468,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$E$20</v>
@@ -4490,7 +4496,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$f$19</v>
@@ -4518,7 +4524,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$f$20</v>
@@ -4546,7 +4552,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$D$6</v>
@@ -4574,7 +4580,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$E$15</v>
@@ -4602,7 +4608,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$E$16</v>
@@ -4630,7 +4636,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$E$28</v>
@@ -4649,7 +4655,7 @@
         <v>121</v>
       </c>
       <c r="F15" s="91">
-        <v>204</v>
+        <v>255</v>
       </c>
       <c r="G15" s="91">
         <v>255</v>
@@ -4658,7 +4664,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$f$28</v>
@@ -4686,7 +4692,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$g$28</v>
@@ -4714,7 +4720,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$E$29</v>
@@ -4742,7 +4748,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$f$29</v>
@@ -4770,7 +4776,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$g$29</v>
@@ -4798,7 +4804,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$f$27</v>
@@ -4826,7 +4832,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$g$27</v>
@@ -4854,7 +4860,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="91" t="str">
         <f>"='"&amp;$D23&amp;"'!"&amp;$E23</f>
         <v>='InputTestData'!$E$27</v>
@@ -4882,7 +4888,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="91" t="str">
         <f>"='"&amp;$D24&amp;"'!"&amp;$E24</f>
         <v>='InputTestData'!$E$31</v>
@@ -4892,13 +4898,13 @@
         <v>'InputTestData'!RatedPointHeadShutoff</v>
       </c>
       <c r="C24" s="102" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D24" s="95" t="s">
         <v>92</v>
       </c>
       <c r="E24" s="101" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F24" s="91">
         <v>255</v>
@@ -4910,7 +4916,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$E$32</v>
@@ -4938,7 +4944,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$E$30</v>
@@ -4966,7 +4972,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$E$26</v>
@@ -4994,7 +5000,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$E$68:$J$68</v>
@@ -5022,7 +5028,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$E$67:$J$67</v>
@@ -5050,7 +5056,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$E$66:$J$66</v>
@@ -5078,7 +5084,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$E$62:$J$62</v>
@@ -5106,7 +5112,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$E$63:$J$63</v>
@@ -5134,7 +5140,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$E$61:$J$61</v>
@@ -5162,7 +5168,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$E$65:$J$65</v>
@@ -5190,7 +5196,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$E$64:$J$64</v>
@@ -5218,7 +5224,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$E$60:$J$60</v>
@@ -5246,7 +5252,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$E$53:$J$53</v>
@@ -5274,7 +5280,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$E$54:$J$54</v>
@@ -5302,7 +5308,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$E$52:$J$52</v>
@@ -5330,7 +5336,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$E$56:$J$56</v>
@@ -5358,7 +5364,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$E$55:$J$55</v>
@@ -5386,7 +5392,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$E$50:$J$50</v>
@@ -5414,7 +5420,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$E$51:$J$51</v>
@@ -5442,7 +5448,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$E$49:$J$49</v>
@@ -5470,7 +5476,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$J$15</v>
@@ -5498,7 +5504,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$e$21</v>
@@ -5526,7 +5532,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="91" t="str">
         <f t="shared" si="0"/>
         <v>='InputTestData'!$f$21</v>
@@ -5564,104 +5570,117 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1EEA0A-3457-1B47-B20D-19D62C1D67E8}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" style="91" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="91"/>
+    <col min="1" max="1" width="27.36328125" style="91" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.81640625" style="91"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="91" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="91" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="91" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="102" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="91" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="102" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="91" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" s="91" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" s="91" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="91" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="91" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="91" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="91" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="91" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="91" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="91" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="91" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" s="91" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="91" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" s="91" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" s="91" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" s="91" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" s="91" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="91" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="91" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="91" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="91" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" s="91" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="91" t="s">
-        <v>200</v>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="91" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="91" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A19">
+    <sortCondition ref="A1:A19"/>
+  </sortState>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -5677,109 +5696,109 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="97" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>216</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>